<commit_message>
comillas simples eliminadas, prompts testing añadidos
</commit_message>
<xml_diff>
--- a/script_master_data_beltran/ficherosExcelOrigen/DED-TESTING_Adopcion IA_v2a_v1.0.xlsx
+++ b/script_master_data_beltran/ficherosExcelOrigen/DED-TESTING_Adopcion IA_v2a_v1.0.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24332"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEF5834C-8A32-42F6-B076-344D1F93B52B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE70E869-FFD6-4096-B3F8-78F3DF515C29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -57,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2691" uniqueCount="319">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2691" uniqueCount="312">
   <si>
     <t>GISS-DED - Adopción IA: &lt;Testing&gt;</t>
   </si>
@@ -1016,27 +1016,6 @@
   <si>
     <t>prompts</t>
   </si>
-  <si>
-    <t>Crear HU</t>
-  </si>
-  <si>
-    <t>Documentar</t>
-  </si>
-  <si>
-    <t>Refactorizar</t>
-  </si>
-  <si>
-    <t>Comprender Codigo Fuente</t>
-  </si>
-  <si>
-    <t>Analisis Desa APIs</t>
-  </si>
-  <si>
-    <t>Pruebas Unitarias</t>
-  </si>
-  <si>
-    <t>Pruebas Funcionales</t>
-  </si>
 </sst>
 </file>
 
@@ -1155,13 +1134,12 @@
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial Narrow"/>
-      <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="9"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
-      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -20835,10 +20813,10 @@
   <dimension ref="B1:BR196"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="4" ySplit="5" topLeftCell="AL6" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="5" topLeftCell="AK6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="AS5" sqref="AS5:AS12"/>
+      <selection pane="bottomRight" activeCell="AS12" sqref="AS12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -20953,7 +20931,7 @@
       <c r="AO4" s="147"/>
       <c r="AP4" s="125"/>
     </row>
-    <row r="5" spans="2:45" ht="39.5" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:45" ht="39" x14ac:dyDescent="0.3">
       <c r="B5" s="3" t="s">
         <v>9</v>
       </c>
@@ -21083,11 +21061,11 @@
       <c r="AR5" s="21" t="s">
         <v>21</v>
       </c>
-      <c r="AS5" t="s">
+      <c r="AS5" s="1" t="s">
         <v>311</v>
       </c>
     </row>
-    <row r="6" spans="2:45" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:45" ht="13" x14ac:dyDescent="0.3">
       <c r="B6" s="5" t="s">
         <v>22</v>
       </c>
@@ -21219,11 +21197,11 @@
         <f>IF(B6="","",IF(OR(H6="S",M6="S",R6="S",W6="S",AB6="S",AG6="S",AL6="S"),"S","N"))</f>
         <v>S</v>
       </c>
-      <c r="AS6" t="s">
-        <v>312</v>
+      <c r="AS6" s="1" t="s">
+        <v>2</v>
       </c>
     </row>
-    <row r="7" spans="2:45" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:45" ht="13" x14ac:dyDescent="0.3">
       <c r="B7" s="5" t="s">
         <v>22</v>
       </c>
@@ -21355,11 +21333,11 @@
         <f t="shared" ref="AR7:AR70" si="1">IF(B7="","",IF(OR(H7="S",M7="S",R7="S",W7="S",AB7="S",AG7="S",AL7="S"),"S","N"))</f>
         <v>S</v>
       </c>
-      <c r="AS7" t="s">
-        <v>313</v>
+      <c r="AS7" s="1" t="s">
+        <v>3</v>
       </c>
     </row>
-    <row r="8" spans="2:45" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:45" ht="13" x14ac:dyDescent="0.3">
       <c r="B8" s="5" t="s">
         <v>22</v>
       </c>
@@ -21491,11 +21469,11 @@
         <f t="shared" si="1"/>
         <v>S</v>
       </c>
-      <c r="AS8" t="s">
-        <v>314</v>
+      <c r="AS8" s="1" t="s">
+        <v>4</v>
       </c>
     </row>
-    <row r="9" spans="2:45" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:45" ht="13" x14ac:dyDescent="0.3">
       <c r="B9" s="5" t="s">
         <v>22</v>
       </c>
@@ -21627,11 +21605,11 @@
         <f t="shared" si="1"/>
         <v>S</v>
       </c>
-      <c r="AS9" t="s">
-        <v>315</v>
+      <c r="AS9" s="1" t="s">
+        <v>5</v>
       </c>
     </row>
-    <row r="10" spans="2:45" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:45" ht="13" x14ac:dyDescent="0.3">
       <c r="B10" s="5" t="s">
         <v>22</v>
       </c>
@@ -21763,11 +21741,11 @@
         <f t="shared" si="1"/>
         <v>S</v>
       </c>
-      <c r="AS10" t="s">
-        <v>316</v>
+      <c r="AS10" s="1" t="s">
+        <v>6</v>
       </c>
     </row>
-    <row r="11" spans="2:45" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:45" ht="13" x14ac:dyDescent="0.3">
       <c r="B11" s="5" t="s">
         <v>40</v>
       </c>
@@ -21899,11 +21877,11 @@
         <f t="shared" si="1"/>
         <v>S</v>
       </c>
-      <c r="AS11" t="s">
-        <v>317</v>
+      <c r="AS11" s="1" t="s">
+        <v>7</v>
       </c>
     </row>
-    <row r="12" spans="2:45" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:45" ht="13" x14ac:dyDescent="0.3">
       <c r="B12" s="5" t="s">
         <v>40</v>
       </c>
@@ -22035,8 +22013,8 @@
         <f t="shared" si="1"/>
         <v>S</v>
       </c>
-      <c r="AS12" t="s">
-        <v>318</v>
+      <c r="AS12" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="13" spans="2:45" ht="13" x14ac:dyDescent="0.3">
@@ -43879,6 +43857,20 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <SharedWithUsers xmlns="c3e1b4bb-9124-477c-aa49-683b9a26b58f">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </SharedWithUsers>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100E080B9D539EE5249B0F7896E1534F47F" ma:contentTypeVersion="10" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="1a88378f58b9ad7590fd740332c19a90">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="8c298b4c-1b69-4120-abb9-a44ffc4bda23" xmlns:ns3="c3e1b4bb-9124-477c-aa49-683b9a26b58f" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="910b3ddf48a2c6cdf16d80fb4d738ee7" ns2:_="" ns3:_="">
     <xsd:import namespace="8c298b4c-1b69-4120-abb9-a44ffc4bda23"/>
@@ -44079,7 +44071,7 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -44088,21 +44080,17 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <SharedWithUsers xmlns="c3e1b4bb-9124-477c-aa49-683b9a26b58f">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </SharedWithUsers>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8E2FEBBB-B4B0-4147-BA7E-181AD49E4B6A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="c3e1b4bb-9124-477c-aa49-683b9a26b58f"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{749E22C5-4A50-411E-A267-99434988BB08}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -44121,20 +44109,10 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{890994BF-65F0-45C5-A04B-1A065C31A5EA}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8E2FEBBB-B4B0-4147-BA7E-181AD49E4B6A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="c3e1b4bb-9124-477c-aa49-683b9a26b58f"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>